<commit_message>
version to read several columns
</commit_message>
<xml_diff>
--- a/TESTI.xlsx
+++ b/TESTI.xlsx
@@ -24,18 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
-  <si>
-    <t>_449-arvo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>vartio</t>
-  </si>
-  <si>
-    <t>tulos</t>
-  </si>
-  <si>
-    <t>tag</t>
   </si>
 </sst>
 </file>
@@ -390,20 +381,20 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>449</v>
+      </c>
+      <c r="C1">
+        <v>450</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -413,7 +404,7 @@
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
         <v>0</v>
       </c>
     </row>
@@ -424,8 +415,8 @@
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>0</v>
+      <c r="C3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saving fixed, input values converted to str before sending
</commit_message>
<xml_diff>
--- a/TESTI.xlsx
+++ b/TESTI.xlsx
@@ -33,6 +33,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="168" formatCode="[h]:mm:ss;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -62,8 +66,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -381,42 +388,45 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>449</v>
+      <c r="B1" s="2">
+        <v>778</v>
       </c>
       <c r="C1">
-        <v>450</v>
+        <v>777</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
+      <c r="B2" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.47916666666666669</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>42</v>
       </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
+      <c r="B3" s="3">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.90277777777777779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>